<commit_message>
Fixed template names, updated tests templates and fixed project_link_sample tests
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_4_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F01A70-E005-D046-ABEF-023C6B8D02E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457F4C92-6455-7A41-A910-C4957AA53037}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleSubmission" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="U7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="V7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -40,10 +40,37 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>======
-ID#AAAAJQGvpsY
-ALEXANDRE BELISLE    (2020-03-30 21:12:07)
-If Nucleic Acic</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAAJQGvpsY
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ALEXANDRE BELISLE    (2020-03-30 21:12:07)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>If Nucleic Acic</t>
         </r>
       </text>
     </comment>
@@ -1925,9 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1936,14 +1961,15 @@
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="8" max="9" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" customWidth="1"/>
@@ -2025,67 +2051,67 @@
         <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="T7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="U7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="V7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="W7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="X7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="X7" s="6" t="s">
+      <c r="Y7" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.2">
@@ -2130,7 +2156,6 @@
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
       <c r="N9" s="7"/>
@@ -2218,7 +2243,6 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="N12" s="7"/>
       <c r="O12" s="8"/>
@@ -18097,31 +18121,23 @@
       <c r="V1000" s="2"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No valid Data" sqref="G9:G391" xr:uid="{33FEAEA0-C2A2-F74A-8AE0-4F7C06A64195}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{F780FD2B-5F2B-124B-9A35-C2A2F76BDFE6}">
           <x14:formula1>
-            <xm:f>Index!$D$2:$D$4</xm:f>
+            <xm:f>Index!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
           <xm:sqref>H8:H391</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>Index!$E$2:$E$4</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>N8:N391</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{A3AD61E6-D8B6-F745-BF26-B8F1F88518C7}">
           <x14:formula1>
             <xm:f>Index!$C$2:$C$12</xm:f>
           </x14:formula1>
@@ -18130,34 +18146,7 @@
           </x14:formula2>
           <xm:sqref>B8:B391</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No valid Data" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>Index!$G$2:$G$4</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>G8:G391</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>Index!$H$2:$H$14</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>U8:U391</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Coordinate" xr:uid="{00000000-0002-0000-0000-000005000000}">
-          <x14:formula1>
-            <xm:f>IF(OR($H8="Tube",$H8="96-well plate"),Index!$A$2:$A$97,IF($H8="384-well plate",Index!$B$2:$B$385,""))</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>L8:L391</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
+        <x14:dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2806ECB-44DC-E44D-9A31-26E80D0A5255}">
           <x14:formula1>
             <xm:f>Index!$F$2:$F$4</xm:f>
           </x14:formula1>
@@ -18165,6 +18154,30 @@
             <xm:f>0</xm:f>
           </x14:formula2>
           <xm:sqref>T8:T391</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8639239A-8304-EB41-9015-10BAF83925F9}">
+          <x14:formula1>
+            <xm:f>Index!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I8:I391</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Coordinate" xr:uid="{FA2826C9-897E-9D4F-9D71-FF3A6B1F3BB7}">
+          <x14:formula1>
+            <xm:f>IF(OR($I8="Tube",$I8="96-well plate"),Index!$A$2:$A$97,IF($I8="384-well plate",Index!$B$2:$B$385,""))</xm:f>
+          </x14:formula1>
+          <xm:sqref>M8:M391</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C82E0352-0208-0F4C-BF36-321A48B3873E}">
+          <x14:formula1>
+            <xm:f>Index!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>O8:O391</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D637506-4C5A-0449-8827-67177805FB67}">
+          <x14:formula1>
+            <xm:f>Index!$H$2:$H$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>V8:V391</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18176,7 +18189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>